<commit_message>
added skin reactions files and code for extract images from pdf
</commit_message>
<xml_diff>
--- a/work_with_prepared_data/datas/P_25.6_n_2.56_2019.xlsx
+++ b/work_with_prepared_data/datas/P_25.6_n_2.56_2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Kizilova\Крысы сканы\N+P\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scripts\neuro_stats\work_with_prepared_data\datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -149,9 +149,6 @@
     <t>2,5 - 1,7 - 1,0</t>
   </si>
   <si>
-    <t>1,4 - 1, 5 - 0,8</t>
-  </si>
-  <si>
     <t>1,6 - 1,4 - 0,9</t>
   </si>
   <si>
@@ -279,6 +276,9 @@
   </si>
   <si>
     <t>2,5 - 2,1 - 1,4</t>
+  </si>
+  <si>
+    <t>1,4 - 1,5 - 0,8</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,22 +675,22 @@
         <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -707,22 +707,22 @@
         <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -739,22 +739,22 @@
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -768,25 +768,25 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" t="s">
         <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -800,25 +800,25 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -832,25 +832,25 @@
         <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -873,16 +873,16 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -896,25 +896,25 @@
         <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>